<commit_message>
Home task 8. Some fix to task 6 and 7
</commit_message>
<xml_diff>
--- a/src/test/kotlin/ru/tilman/algorithms/task6/compare.xlsx
+++ b/src/test/kotlin/ru/tilman/algorithms/task6/compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/18515002/Documents/develop/dailychallenge/src/test/kotlin/ru/tilman/algorithms/task6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AEDDF3-6CC9-224E-BD70-88EBB796B412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6428865-A65B-B64E-AD8B-D178175F6834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32700" yWindow="5580" windowWidth="37940" windowHeight="28080" xr2:uid="{722AF461-8D03-A548-BC90-9570DEE73DC2}"/>
+    <workbookView xWindow="34520" yWindow="3280" windowWidth="37940" windowHeight="28080" xr2:uid="{722AF461-8D03-A548-BC90-9570DEE73DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>-</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>№</t>
+  </si>
+  <si>
+    <t>MergeSort (manyTempArr)</t>
+  </si>
+  <si>
+    <t>MergeSort (singleTempArr)</t>
+  </si>
+  <si>
+    <t>Qsort</t>
   </si>
 </sst>
 </file>
@@ -136,34 +145,28 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -231,6 +234,12 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -273,17 +282,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F07C4D3-649D-8940-AAA5-AB46AB1CD94C}" name="Таблица1" displayName="Таблица1" ref="A1:H8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0">
-  <autoFilter ref="A1:H8" xr:uid="{0F07C4D3-649D-8940-AAA5-AB46AB1CD94C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F07C4D3-649D-8940-AAA5-AB46AB1CD94C}" name="Таблица1" displayName="Таблица1" ref="A1:H11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H11" xr:uid="{0F07C4D3-649D-8940-AAA5-AB46AB1CD94C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3250DB0D-E900-FF4E-BE75-881940CC7A69}" name="№" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{AEA81493-3A1D-7347-9753-5A9AE262DC7E}" name="Алгоритм\tSort, ms" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3E2D4C83-5D3D-5B46-A4E6-5F9FD78109E0}" name="100" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{5C9D53D7-8C23-6B4D-8BAA-642AD34FE368}" name="1 000" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1941CFFD-1259-A043-A863-1C95CC1AD0CC}" name="10 000" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C87E764B-D452-C54E-9E35-A937B326D309}" name="100 000" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{34A690D5-037C-1240-9A3A-66035DB9D4B8}" name="1 000 000" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{DA263A52-7761-9844-A540-7431E5DFFAD2}" name="10 000 000" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3250DB0D-E900-FF4E-BE75-881940CC7A69}" name="№" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AEA81493-3A1D-7347-9753-5A9AE262DC7E}" name="Алгоритм\tSort, ms" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{3E2D4C83-5D3D-5B46-A4E6-5F9FD78109E0}" name="100" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5C9D53D7-8C23-6B4D-8BAA-642AD34FE368}" name="1 000" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1941CFFD-1259-A043-A863-1C95CC1AD0CC}" name="10 000" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C87E764B-D452-C54E-9E35-A937B326D309}" name="100 000" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{34A690D5-037C-1240-9A3A-66035DB9D4B8}" name="1 000 000" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{DA263A52-7761-9844-A540-7431E5DFFAD2}" name="10 000 000" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,16 +595,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80D133-7A9E-1242-AF5F-51FF51B04D1E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D22" sqref="A18:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
@@ -605,252 +614,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>38</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>876</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>110806</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>24</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>675</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>101303</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
         <v>17</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>631</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>43562</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>16</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>338</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>52898</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>13</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>165</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>3103</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>62479</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>7</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>50</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>599</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>81636</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>11</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>157</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>1748</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>25728</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6">
+        <v>53</v>
+      </c>
+      <c r="G9" s="6">
+        <v>830</v>
+      </c>
+      <c r="H9" s="6">
+        <v>12562</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6">
+        <v>35</v>
+      </c>
+      <c r="G10" s="6">
+        <v>741</v>
+      </c>
+      <c r="H10" s="6">
+        <v>10872</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1028</v>
+      </c>
+      <c r="H11" s="6">
+        <v>14161</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>